<commit_message>
Apache POI with excel
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taieb/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertek/IdeaProjects/SdetFastTrackCucumber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D687CE1-B578-F548-B3D2-0A50B17B7A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA75C340-CD0C-5740-B049-7B855A3C5CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4B3AB7B9-7EAA-E548-AB48-F6CBC4BFEF3C}"/>
+    <workbookView minimized="1" xWindow="10480" yWindow="2480" windowWidth="18500" windowHeight="13880" xr2:uid="{686346D6-ACEE-E947-A699-24BFDEEC9EBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,9 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>FirstName</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+  <si>
+    <t>Firstname</t>
   </si>
   <si>
     <t>LastName</t>
@@ -49,43 +48,53 @@
     <t>Mary</t>
   </si>
   <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Vinod</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Mansoor</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>SDET</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
     <t>Jones</t>
   </si>
   <si>
-    <t>PO</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>ali</t>
-  </si>
-  <si>
-    <t>Mohamed</t>
-  </si>
-  <si>
-    <t>Hassan</t>
-  </si>
-  <si>
-    <t>ouberka</t>
-  </si>
-  <si>
-    <t>Linda</t>
-  </si>
-  <si>
     <t>Smith</t>
-  </si>
-  <si>
-    <t>SDET</t>
-  </si>
-  <si>
-    <t>Developer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -95,21 +104,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -117,31 +120,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,73 +439,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6348AE18-7591-9C4D-B85D-C9B498BE60E9}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE25B705-A0AD-0542-B6B1-9715AD38153E}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="364" zoomScaleNormal="364" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>200000.0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
+      <c r="D3" t="n">
+        <v>110000.0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="n">
+        <v>135000.0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="n">
+        <v>125000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>